<commit_message>
add day 0 exercises + day 1 : ex. 1 to 3
</commit_message>
<xml_diff>
--- a/data/Malaria_Dataset_Key.xlsx
+++ b/data/Malaria_Dataset_Key.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\KU\Teaching\DataVizCourse\2024\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28A9FDC1-6C13-40E9-94DF-ADD664C72E8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet2" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="57">
   <si>
     <t xml:space="preserve">Column </t>
   </si>
@@ -179,30 +188,35 @@
   </si>
   <si>
     <t>Distance to cities with population &gt; 50000</t>
+  </si>
+  <si>
+    <t>Brightness of night time lights in that location (arbitrary scale). Defined in https://pophealthmetrics.biomedcentral.com/articles/10.1186/1478-7954-6-5#Sec10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="&quot;Aptos Narrow&quot;"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="&quot;Arial&quot;"/>
     </font>
@@ -212,42 +226,45 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -437,23 +454,28 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:B35"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="34.0"/>
+    <col min="1" max="1" width="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -461,47 +483,47 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:2">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:2">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:2">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:2">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:2">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:2">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:2">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -509,7 +531,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:2">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
@@ -517,7 +539,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:2">
       <c r="A12" s="2" t="s">
         <v>14</v>
       </c>
@@ -525,12 +547,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:2">
       <c r="A13" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:2">
       <c r="A14" s="2" t="s">
         <v>17</v>
       </c>
@@ -538,7 +560,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:2">
       <c r="A15" s="2" t="s">
         <v>19</v>
       </c>
@@ -546,7 +568,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:2">
       <c r="A16" s="2" t="s">
         <v>20</v>
       </c>
@@ -554,7 +576,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:2">
       <c r="A17" s="2" t="s">
         <v>22</v>
       </c>
@@ -562,7 +584,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:2">
       <c r="A18" s="2" t="s">
         <v>24</v>
       </c>
@@ -570,7 +592,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:2">
       <c r="A19" s="2" t="s">
         <v>26</v>
       </c>
@@ -578,17 +600,17 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:2">
       <c r="A20" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:2">
       <c r="A21" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:2">
       <c r="A22" s="2" t="s">
         <v>30</v>
       </c>
@@ -596,7 +618,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:2">
       <c r="A23" s="2" t="s">
         <v>32</v>
       </c>
@@ -604,7 +626,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:2">
       <c r="A24" s="2" t="s">
         <v>34</v>
       </c>
@@ -612,7 +634,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:2">
       <c r="A25" s="2" t="s">
         <v>36</v>
       </c>
@@ -620,7 +642,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:2">
       <c r="A26" s="2" t="s">
         <v>38</v>
       </c>
@@ -628,7 +650,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:2">
       <c r="A27" s="2" t="s">
         <v>40</v>
       </c>
@@ -636,7 +658,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:2">
       <c r="A28" s="2" t="s">
         <v>42</v>
       </c>
@@ -644,7 +666,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:2">
       <c r="A29" s="2" t="s">
         <v>44</v>
       </c>
@@ -652,12 +674,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:2">
       <c r="A30" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:2">
       <c r="A31" s="2" t="s">
         <v>47</v>
       </c>
@@ -665,7 +687,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:2">
       <c r="A32" s="2" t="s">
         <v>49</v>
       </c>
@@ -673,7 +695,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:2">
       <c r="A33" s="2" t="s">
         <v>51</v>
       </c>
@@ -681,12 +703,15 @@
         <v>52</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:2">
       <c r="A34" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="35">
+      <c r="B34" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
       <c r="A35" s="2" t="s">
         <v>54</v>
       </c>
@@ -695,6 +720,6 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Exercises : day 1 complete
</commit_message>
<xml_diff>
--- a/data/Malaria_Dataset_Key.xlsx
+++ b/data/Malaria_Dataset_Key.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\KU\Teaching\DataVizCourse\2024\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28A9FDC1-6C13-40E9-94DF-ADD664C72E8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39291183-8966-4AF5-B70A-87189CD3311A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="16680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="1" r:id="rId1"/>
@@ -112,9 +112,6 @@
     <t>dhs_survey_id</t>
   </si>
   <si>
-    <t>itnuse</t>
-  </si>
-  <si>
     <t>Insecticide-treated bed nets type 0</t>
   </si>
   <si>
@@ -160,18 +157,12 @@
     <t>Land reflectance brightness</t>
   </si>
   <si>
-    <t>mosquito_temperature_suitability</t>
-  </si>
-  <si>
     <t>precipitation</t>
   </si>
   <si>
     <t>Precipitation in the 10km^2 radius</t>
   </si>
   <si>
-    <t>enhanced_vegitation_index</t>
-  </si>
-  <si>
     <t>Calculated vegetation index</t>
   </si>
   <si>
@@ -191,6 +182,15 @@
   </si>
   <si>
     <t>Brightness of night time lights in that location (arbitrary scale). Defined in https://pophealthmetrics.biomedcentral.com/articles/10.1186/1478-7954-6-5#Sec10</t>
+  </si>
+  <si>
+    <t>enhanced_vegetation_index</t>
+  </si>
+  <si>
+    <t>itnuse0</t>
+  </si>
+  <si>
+    <t>mosquito_temperature_suitability_index</t>
   </si>
 </sst>
 </file>
@@ -466,13 +466,13 @@
   </sheetPr>
   <dimension ref="A1:B35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="34" customWidth="1"/>
+    <col min="1" max="1" width="36.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -612,111 +612,111 @@
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="2" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="2" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update Malaria dataset key
</commit_message>
<xml_diff>
--- a/data/Malaria_Dataset_Key.xlsx
+++ b/data/Malaria_Dataset_Key.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\KU\Teaching\DataVizCourse\2024\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39291183-8966-4AF5-B70A-87189CD3311A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EDCD382-5F5D-49E2-AA7D-2606D7FDBBD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="16680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="58">
   <si>
     <t xml:space="preserve">Column </t>
   </si>
@@ -97,9 +97,6 @@
     <t>PfPr</t>
   </si>
   <si>
-    <t>Plasmodium falciparum parasite rate</t>
-  </si>
-  <si>
     <t>method</t>
   </si>
   <si>
@@ -112,51 +109,27 @@
     <t>dhs_survey_id</t>
   </si>
   <si>
-    <t>Insecticide-treated bed nets type 0</t>
-  </si>
-  <si>
     <t>itnuse1</t>
   </si>
   <si>
-    <t>Insecticide-treated bed nets type 1</t>
-  </si>
-  <si>
     <t>itnuse2</t>
   </si>
   <si>
-    <t>Insecticide-treated bed nets type 2</t>
-  </si>
-  <si>
     <t>itnuse3</t>
   </si>
   <si>
-    <t>Insecticide-treated bed nets type 3</t>
-  </si>
-  <si>
     <t>itnavg4</t>
   </si>
   <si>
-    <t>Average Insecticide-treated bed nets usage</t>
-  </si>
-  <si>
     <t>act</t>
   </si>
   <si>
-    <t>Artemisinin-based combination therapies</t>
-  </si>
-  <si>
     <t>irs</t>
   </si>
   <si>
-    <t>Indoor Residual Spraying</t>
-  </si>
-  <si>
     <t>tasseled_cap_wetness</t>
   </si>
   <si>
-    <t>Land reflectance brightness</t>
-  </si>
-  <si>
     <t>precipitation</t>
   </si>
   <si>
@@ -181,9 +154,6 @@
     <t>Distance to cities with population &gt; 50000</t>
   </si>
   <si>
-    <t>Brightness of night time lights in that location (arbitrary scale). Defined in https://pophealthmetrics.biomedcentral.com/articles/10.1186/1478-7954-6-5#Sec10</t>
-  </si>
-  <si>
     <t>enhanced_vegetation_index</t>
   </si>
   <si>
@@ -191,13 +161,59 @@
   </si>
   <si>
     <t>mosquito_temperature_suitability_index</t>
+  </si>
+  <si>
+    <t>Insecticide-treated bed nets usage
+Measured as percentage of population with access to an ITN [1,2,3,4,5]</t>
+  </si>
+  <si>
+    <t>Insecticide-treated bed nets
+Measured as percentage of households with at least one ITN for every two persons who stayed in the household the night
+before the survey [1,2,3,4,5]</t>
+  </si>
+  <si>
+    <t>Insecticide-treated bed nets, an effective preventative measure against mosquitoes
+Measured as percentage of households with at least one ITN [1,2,3,4,5]</t>
+  </si>
+  <si>
+    <t>Insecticide-treated bed 
+Measured as percentage of pulation who slept under an ITN last night [1,2,3,4,5]</t>
+  </si>
+  <si>
+    <t>ITN and or Indoor Residual Spraying
+Measured as percentage of households with Indoor Residual Spraying (IRS) in the last 12 months [1,2,3,4,5]</t>
+  </si>
+  <si>
+    <t>Artemisinin-based combination therapies- treatment for malaria. 
+Measured in percentage of children who received any ACT in the past 2 weeks before the survey [1,2,3,4,5]</t>
+  </si>
+  <si>
+    <t>Indoor Residual Spraying
+Measured as percentage of households with Indoor Residual Spraying (IRS) in the last 12 months [1,2,3,4,5]</t>
+  </si>
+  <si>
+    <t>Land reflectance brightness
+Measures the fraction of incoming solar radiation that is reflected from the earth's surface to the LandSat sensor. 
+Ratio of reflected light wavelength vs total light wavelength. No unit (6)</t>
+  </si>
+  <si>
+    <t>Mosquito temperature suitability
+Range of 15.3C to 31.2C [7]</t>
+  </si>
+  <si>
+    <t>Brightness of nighttime lights in that location
+Measured on an arbitrary scale, used as a proxy for poverty [7]</t>
+  </si>
+  <si>
+    <t>Plasmodium falciparum parasite rate
+Calculated using log(Npositive*Nexamined+0.5)/log(Nexamined*(1-Npositive)+0.5) (empirical logit formula) [8]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -220,6 +236,13 @@
       <color rgb="FF000000"/>
       <name val="&quot;Arial&quot;"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -241,11 +264,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -466,16 +496,17 @@
   </sheetPr>
   <dimension ref="A1:B35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="36.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="134.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" ht="12.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -483,47 +514,55 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" ht="14.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="B2" s="3"/>
+    </row>
+    <row r="3" spans="1:2" ht="14.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="B3" s="3"/>
+    </row>
+    <row r="4" spans="1:2" ht="14.25">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="B4" s="3"/>
+    </row>
+    <row r="5" spans="1:2" ht="14.25">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="B5" s="3"/>
+    </row>
+    <row r="6" spans="1:2" ht="14.25">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="B6" s="3"/>
+    </row>
+    <row r="7" spans="1:2" ht="14.25">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
+      <c r="B7" s="3"/>
+    </row>
+    <row r="8" spans="1:2" ht="14.25">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
+      <c r="B8" s="3"/>
+    </row>
+    <row r="9" spans="1:2" ht="14.25">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
+      <c r="B9" s="3"/>
+    </row>
+    <row r="10" spans="1:2" ht="14.25">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -531,7 +570,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" ht="14.25">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
@@ -539,7 +578,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" ht="14.25">
       <c r="A12" s="2" t="s">
         <v>14</v>
       </c>
@@ -547,12 +586,13 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" ht="14.25">
       <c r="A13" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="14" spans="1:2">
+      <c r="B13" s="3"/>
+    </row>
+    <row r="14" spans="1:2" ht="14.25">
       <c r="A14" s="2" t="s">
         <v>17</v>
       </c>
@@ -560,15 +600,15 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" ht="14.25">
       <c r="A15" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" ht="14.25">
       <c r="A16" s="2" t="s">
         <v>20</v>
       </c>
@@ -576,147 +616,152 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" ht="14.25">
       <c r="A17" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" ht="29.25" customHeight="1">
       <c r="A18" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="14.25">
+      <c r="A19" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="2" t="s">
+      <c r="B19" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B19" s="1" t="s">
+    </row>
+    <row r="20" spans="1:2" ht="14.25">
+      <c r="A20" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="2" t="s">
+      <c r="B20" s="3"/>
+    </row>
+    <row r="21" spans="1:2" ht="14.25">
+      <c r="A21" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="2" t="s">
+      <c r="B21" s="3"/>
+    </row>
+    <row r="22" spans="1:2" ht="25.5">
+      <c r="A22" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="38.25">
+      <c r="A23" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="2" t="s">
+      <c r="B23" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="25.5">
+      <c r="A24" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="25.5">
+      <c r="A25" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="25.5">
+      <c r="A26" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="25.5">
+      <c r="A27" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="25.5">
+      <c r="A28" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="38.25">
+      <c r="A29" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="25.5">
+      <c r="A30" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B30" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B25" s="1" t="s">
+    </row>
+    <row r="31" spans="1:2" ht="14.25">
+      <c r="A31" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" s="2" t="s">
+      <c r="B31" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B26" s="1" t="s">
+    </row>
+    <row r="32" spans="1:2" ht="14.25">
+      <c r="A32" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
-      <c r="A27" s="2" t="s">
+    <row r="33" spans="1:2" ht="14.25">
+      <c r="A33" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B33" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
-      <c r="A28" s="2" t="s">
+    <row r="34" spans="1:2" ht="25.5">
+      <c r="A34" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B34" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="14.25">
+      <c r="A35" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29" s="2" t="s">
+      <c r="B35" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2">
-      <c r="A30" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
-      <c r="A31" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
-      <c r="A32" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2">
-      <c r="A33" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2">
-      <c r="A34" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2">
-      <c r="A35" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>